<commit_message>
feat(export): ajout d'une colonne pour indiquer les SMS
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/www/beta/domifa/packages/backend/src/excel/_templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541EC41B-AA98-2140-A21A-63500BA3CE1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12498953-2512-6B43-8657-11BE71DC4010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liste des usagers" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>Date et heure</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Si renouvellement, utilisateur l'ayant validé</t>
+  </si>
+  <si>
+    <t>Notifications SMS</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMO2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U5" sqref="U5"/>
     </sheetView>
@@ -781,11 +784,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK2"/>
+  <dimension ref="A1:AML2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,17 +797,17 @@
     <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
     <col min="3" max="4" width="15.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5" style="1" customWidth="1"/>
-    <col min="13" max="1025" width="8.5" style="1" customWidth="1"/>
+    <col min="6" max="7" width="16.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5" style="1" customWidth="1"/>
+    <col min="14" max="1026" width="8.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -812,7 +815,7 @@
         <v>44125.4504903704</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -832,27 +835,30 @@
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(sms): Mise a jour du guide fix(export): ajout de la colonne numero de distribution
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E40C88-64E7-C84F-9EFA-57DEB55FA877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED71AA42-36F8-6146-B201-F1042DF9B2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>Date et heure</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Indicatif pays</t>
+  </si>
+  <si>
+    <t>Numéro de distribution spéciale (BP, TSA, etc)</t>
   </si>
 </sst>
 </file>
@@ -187,7 +190,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy&quot; à &quot;hh:mm"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="64"/>
@@ -198,6 +201,13 @@
       <sz val="12"/>
       <color indexed="64"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="64"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -220,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -233,6 +243,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,12 +474,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMP2"/>
+  <dimension ref="A1:AMQ2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U5" sqref="U5"/>
-      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,22 +493,23 @@
     <col min="8" max="8" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="52" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="1030" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.83203125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="53" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="1031" width="8.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +517,7 @@
         <v>44125.4504903704</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="3" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" s="3" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -534,46 +548,49 @@
       <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(excel): correction de colonnes du fichier Excel
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4DF80A-F6A9-CA41-97CE-B73DD1817E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0BF477-B00A-ED43-93C7-92B2E6D8F624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liste des usagers" sheetId="1" r:id="rId1"/>
@@ -165,12 +165,6 @@
     <t>Colis distribués</t>
   </si>
   <si>
-    <t>Avis de passage enregistré</t>
-  </si>
-  <si>
-    <t>Avis de passage distribué</t>
-  </si>
-  <si>
     <t>Appels</t>
   </si>
   <si>
@@ -187,6 +181,12 @@
   </si>
   <si>
     <t>Pli non distribuable</t>
+  </si>
+  <si>
+    <t>Avis de passage enregistrés</t>
+  </si>
+  <si>
+    <t>Avis de passage distribués</t>
   </si>
 </sst>
 </file>
@@ -207,6 +207,7 @@
       <sz val="12"/>
       <color indexed="64"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -552,7 +553,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>8</v>
@@ -561,7 +562,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>10</v>
@@ -616,10 +617,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="V6" sqref="V6"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,10 +734,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMN2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H3" sqref="H3"/>
-      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1793,7 +1794,7 @@
       <c r="AMM1" s="4"/>
       <c r="AMN1" s="4"/>
     </row>
-    <row r="2" spans="1:1028" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1028" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1834,22 +1835,22 @@
         <v>46</v>
       </c>
       <c r="N2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="R2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(excel): ajout d'une colonne pour les entretien
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0BF477-B00A-ED43-93C7-92B2E6D8F624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62634C2A-79B4-D04B-97C6-0E3A6C56BC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liste des usagers" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
   <si>
     <t>Date et heure</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Avis de passage distribués</t>
+  </si>
+  <si>
+    <t>Si AUTRE LIEN AVEC LA COMMUNE, précisions</t>
   </si>
 </sst>
 </file>
@@ -615,12 +618,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK2"/>
+  <dimension ref="A1:AML2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="V6" sqref="V6"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,21 +634,22 @@
     <col min="8" max="8" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="43.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="46.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="1025" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="43.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="34.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="46.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="1026" width="14" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +657,7 @@
         <v>44125.4504903704</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -691,36 +695,39 @@
         <v>29</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -734,7 +741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H3" sqref="H3"/>
       <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>

</xml_diff>

<commit_message>
fix(anon): amélioration de l'anonymisation de la préprod feat(manage): ajout de la suppression et radiation de masse des domiciliés fix(rgaa): améliorations des pages d'import, de formulaires
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62634C2A-79B4-D04B-97C6-0E3A6C56BC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3557F338-3899-C441-A985-27E185F70C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liste des usagers" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,6 @@
     <t>Type de domiciliation</t>
   </si>
   <si>
-    <t>Date début dom actuelle</t>
-  </si>
-  <si>
     <t>Date fin de dom</t>
   </si>
   <si>
@@ -190,6 +187,9 @@
   </si>
   <si>
     <t>Si AUTRE LIEN AVEC LA COMMUNE, précisions</t>
+  </si>
+  <si>
+    <t>Date début dom</t>
   </si>
 </sst>
 </file>
@@ -492,10 +492,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMQ2"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U5" sqref="U5"/>
-      <selection pane="bottomLeft" activeCell="V8" sqref="V8"/>
+      <selection pane="bottomLeft" activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,7 +556,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>8</v>
@@ -565,7 +565,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>10</v>
@@ -589,25 +589,25 @@
         <v>16</v>
       </c>
       <c r="S2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -620,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AML2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="V6" sqref="V6"/>
       <selection pane="bottomLeft" activeCell="N4" sqref="N4"/>
@@ -657,7 +657,7 @@
         <v>44125.4504903704</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -677,58 +677,58 @@
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1821,43 +1821,43 @@
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="R2" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(export): add language to excel file
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43C4431-8CF7-0F4E-84C1-B86DB383D6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AA8948-6D1E-D244-9C4E-BCF0D73FB63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liste des usagers" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>Date et heure</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Situation professionnelle</t>
+  </si>
+  <si>
+    <t>Langue parlée</t>
   </si>
 </sst>
 </file>
@@ -490,12 +493,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMQ2"/>
+  <dimension ref="A1:AMR2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U5" sqref="U5"/>
-      <selection pane="bottomLeft" activeCell="U8" sqref="U8"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,23 +512,23 @@
     <col min="8" max="8" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="53" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="1031" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="21.83203125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="54" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="1032" width="8.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +536,7 @@
         <v>44125.4504903704</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="3" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" s="3" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -564,49 +567,52 @@
       <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -745,7 +751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMM2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H3" sqref="H3"/>
       <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
@@ -1803,7 +1809,7 @@
       <c r="AML1" s="4"/>
       <c r="AMM1" s="4"/>
     </row>
-    <row r="2" spans="1:1027" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1027" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
fix(stats): update stats & export
</commit_message>
<xml_diff>
--- a/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
+++ b/packages/backend/src/excel/_templates/export-structure-usagers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/humans/Documents/dev/domifa/packages/backend/src/excel/_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813B6ADD-D048-4547-985B-60CAA69C9834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AED3590-BCE2-0542-99F3-B978088AAA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liste des usagers" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="62">
   <si>
     <t>Date et heure</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Avis de passage réexpédiés</t>
+  </si>
+  <si>
+    <t>Nationalité</t>
   </si>
 </sst>
 </file>
@@ -505,12 +508,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMR2"/>
+  <dimension ref="A1:AMS2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="U5" sqref="U5"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,23 +527,23 @@
     <col min="8" max="8" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="21.83203125" style="1" customWidth="1"/>
-    <col min="13" max="14" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="54" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="1032" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="21.83203125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="55" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="1033" width="8.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +551,7 @@
         <v>44125.4504903704</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="3" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="3" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -582,49 +585,52 @@
       <c r="K2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -638,7 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="V6" sqref="V6"/>
       <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
@@ -1830,7 +1836,7 @@
       <c r="AMO1" s="4"/>
       <c r="AMP1" s="4"/>
     </row>
-    <row r="2" spans="1:1030" s="3" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1030" s="3" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>

</xml_diff>